<commit_message>
added message box (basic)
</commit_message>
<xml_diff>
--- a/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
+++ b/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdomj\source\repos\ExcelLoaderToolForAccounting\TestApp\bin\Debug\net6.0\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felhasználó\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA147124-DACC-4384-B601-1827306D0D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B5C85D-4A82-407A-95C6-9CDACB909804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terv-tény" sheetId="2" r:id="rId1"/>
@@ -13817,7 +13817,7 @@
       <selection activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-      <autoFilter ref="A3:L77" xr:uid="{25633CEA-EAA3-4F51-A5A0-A88B4FC40698}"/>
+      <autoFilter ref="A3:L77" xr:uid="{45470FCE-DAA7-4FBC-B1BE-B8C81F2DBE52}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -31947,9 +31947,9 @@
   <sheetPr codeName="Munka2"/>
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -33014,7 +33014,7 @@
       <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A4:AV400" xr:uid="{5AFC0C04-75FB-41C2-B51E-F7D0439F8612}">
+      <autoFilter ref="A4:AV400" xr:uid="{5AFFAB88-3FB6-4120-ABCF-90DFF735365D}">
         <filterColumn colId="6">
           <filters>
             <filter val="2019.06"/>
@@ -36772,7 +36772,7 @@
       <selection activeCell="L44" sqref="L44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A41:N455" xr:uid="{ABF0025B-BA04-41FF-9769-509F452827AF}"/>
+      <autoFilter ref="A41:N455" xr:uid="{48CBA8F8-4CCE-43F9-81FB-F4EB44779097}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -51719,7 +51719,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="935" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="935" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A935" s="219" t="s">
         <v>801</v>
       </c>
@@ -51740,7 +51740,7 @@
     <row r="939" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A939" s="220"/>
     </row>
-    <row r="940" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A940" s="219" t="s">
         <v>804</v>
       </c>

</xml_diff>

<commit_message>
Added FEJ file creation
</commit_message>
<xml_diff>
--- a/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
+++ b/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felhasználó\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdomj\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4463D44F-361C-4B16-9AB4-F4E359D80691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD232D0-5C69-4D7E-BBE6-690EE2735A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terv-tény" sheetId="2" r:id="rId1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8926" uniqueCount="2704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8937" uniqueCount="2704">
   <si>
     <t>Fennmaradó 
 egyenleg</t>
@@ -12585,11 +12585,11 @@
       </c>
       <c r="E3" s="295">
         <f>SUMIFS(Bérköltség!$B$2:$B$17,Bérköltség!$K$2:$K$17,$C3,Bérköltség!$N$2:$N$17,"Tény")+SUMIFS(Bérköltség!$C$2:$C$17,Bérköltség!$K$2:$K$17,$C3,Bérköltség!$N$2:$N$17,"Tény")</f>
-        <v>352398</v>
+        <v>465898</v>
       </c>
       <c r="F3" s="295">
         <f>D3-E3</f>
-        <v>460359902</v>
+        <v>460246402</v>
       </c>
       <c r="G3" s="295">
         <f>SUMIFS(Bérköltség!$B$2:$B$17,Bérköltség!$K$2:$K$17,$C3,Bérköltség!$N$2:$N$17,"Köt.váll")+SUMIFS(Bérköltség!$C$2:$C$17,Bérköltség!$K$2:$K$17,$C3,Bérköltség!$N$2:$N$17,"Köt.váll")</f>
@@ -12597,7 +12597,7 @@
       </c>
       <c r="H3" s="133">
         <f>F3-G3</f>
-        <v>458325902</v>
+        <v>458212402</v>
       </c>
       <c r="J3" s="110" t="s">
         <v>129</v>
@@ -12611,11 +12611,11 @@
       </c>
       <c r="M3" s="112">
         <f>SUMIFS(Bérköltség!$B$2:$B$17,Bérköltség!$I$2:$I$17,$K3,Bérköltség!$N$2:$N$17,"Tény")+SUMIFS(Bérköltség!$C$2:$C$17,Bérköltség!$I$2:$I$17,$K3,Bérköltség!$N$2:$N$17,"Tény")+SUMIFS(Dologi_felhalm.!$I$3:$I$84,Dologi_felhalm.!$L$3:$L$84,$K3,Dologi_felhalm.!$J$3:$J$84,"Tény")</f>
-        <v>1250649</v>
+        <v>1364149</v>
       </c>
       <c r="N3" s="112">
         <f>L3-M3</f>
-        <v>240493119</v>
+        <v>240379619</v>
       </c>
       <c r="O3" s="112">
         <f>SUMIFS(Bérköltség!$B$2:$B$17,Bérköltség!$I$2:$I$17,$K3,Bérköltség!$N$2:$N$17,"Köt.váll")+SUMIFS(Bérköltség!$C$2:$C$17,Bérköltség!$I$2:$I$17,$K3,Bérköltség!$N$2:$N$17,"Köt.váll")+SUMIFS(Dologi_felhalm.!$I$3:$I$84,Dologi_felhalm.!$L$3:$L$84,$K3,Dologi_felhalm.!$J$3:$J$84,"Köt.váll")</f>
@@ -12623,7 +12623,7 @@
       </c>
       <c r="P3" s="113">
         <f>N3-O3</f>
-        <v>232230681</v>
+        <v>232117181</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -12889,11 +12889,11 @@
       </c>
       <c r="M8" s="125">
         <f t="shared" ref="M8:P8" si="4">SUM(M3:M7)</f>
-        <v>10411901</v>
+        <v>10525401</v>
       </c>
       <c r="N8" s="125">
         <f t="shared" si="4"/>
-        <v>859588099</v>
+        <v>859474599</v>
       </c>
       <c r="O8" s="125">
         <f t="shared" si="4"/>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="P8" s="126">
         <f t="shared" si="4"/>
-        <v>849416453</v>
+        <v>849302953</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13069,11 +13069,11 @@
       </c>
       <c r="L12" s="168">
         <f t="shared" ref="L12:O12" si="5">SUM(E25)</f>
-        <v>9188587</v>
+        <v>9302087</v>
       </c>
       <c r="M12" s="167">
         <f t="shared" si="5"/>
-        <v>785236448</v>
+        <v>785122948</v>
       </c>
       <c r="N12" s="167">
         <f t="shared" si="5"/>
@@ -13081,7 +13081,7 @@
       </c>
       <c r="O12" s="169">
         <f t="shared" si="5"/>
-        <v>775405385</v>
+        <v>775291885</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -13178,11 +13178,11 @@
       </c>
       <c r="L14" s="293">
         <f t="shared" ref="L14:O14" si="7">SUM(L12:L13)</f>
-        <v>10411901</v>
+        <v>10525401</v>
       </c>
       <c r="M14" s="109">
         <f t="shared" si="7"/>
-        <v>859588099</v>
+        <v>859474599</v>
       </c>
       <c r="N14" s="293">
         <f t="shared" si="7"/>
@@ -13190,7 +13190,7 @@
       </c>
       <c r="O14" s="294">
         <f t="shared" si="7"/>
-        <v>849416453</v>
+        <v>849302953</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
@@ -13516,11 +13516,11 @@
       </c>
       <c r="E25" s="58">
         <f t="shared" ref="E25:H25" si="8">SUM(E3:E24)</f>
-        <v>9188587</v>
+        <v>9302087</v>
       </c>
       <c r="F25" s="58">
         <f t="shared" si="8"/>
-        <v>785236448</v>
+        <v>785122948</v>
       </c>
       <c r="G25" s="58">
         <f t="shared" si="8"/>
@@ -13528,7 +13528,7 @@
       </c>
       <c r="H25" s="58">
         <f t="shared" si="8"/>
-        <v>775405385</v>
+        <v>775291885</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -13817,7 +13817,7 @@
       <selection activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-      <autoFilter ref="A3:L77" xr:uid="{EE3C3F08-645C-4296-99D4-DFA922CC3AF5}"/>
+      <autoFilter ref="A3:L77" xr:uid="{FFF0F522-7073-4465-B389-2F7F5F865305}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -31947,9 +31947,9 @@
   <sheetPr codeName="Munka2"/>
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -32682,42 +32682,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="290"/>
-      <c r="B10" s="256"/>
-      <c r="C10" s="256"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="108"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="121"/>
-      <c r="Q10" s="122"/>
-      <c r="R10" s="116"/>
-      <c r="S10" s="116"/>
-      <c r="T10" s="117"/>
-      <c r="U10" s="123" t="str">
-        <f t="shared" ref="U10:U12" si="22">IFERROR(ROUND(P10*S10/R10,0),"")</f>
-        <v/>
-      </c>
-      <c r="V10" s="123" t="str">
-        <f t="shared" ref="V10:V12" si="23">IFERROR(ROUND(U10*X10,0),"")</f>
-        <v/>
-      </c>
-      <c r="W10" s="118"/>
+    <row r="10" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="291" t="e">
+        <f>IF(#REF!="FEOR",#REF!,IF(#REF!="HIÁNYOS ADATOK","HIÁNYOS ADATOK",#REF!))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B10" s="256">
+        <v>100000</v>
+      </c>
+      <c r="C10" s="256">
+        <v>13500</v>
+      </c>
+      <c r="D10" s="10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="236">
+        <v>8346442386</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>1215</v>
+      </c>
+      <c r="G10" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="81" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="108" t="str">
+        <f>IF(COUNTIFS(Admin!$A$29:$A$40,L10)&gt;0,Admin!$A$28,IF(COUNTIFS(Admin!$B$29:$B$40,L10)&gt;0,Admin!$B$28,IF(COUNTIFS(Admin!$C$29:$C$40,L10)&gt;0,Admin!$C$28,IF(COUNTIFS(Admin!$D$29:$D$40,L10)&gt;0,Admin!$D$28,"-"))))</f>
+        <v>2. mérföldkő</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" s="121">
+        <v>1373700</v>
+      </c>
+      <c r="Q10" s="122">
+        <f t="shared" ref="Q10" si="22">IFERROR(ROUND(P10*X10,0),"")</f>
+        <v>178581</v>
+      </c>
+      <c r="R10" s="116">
+        <v>174</v>
+      </c>
+      <c r="S10" s="116">
+        <v>37</v>
+      </c>
+      <c r="T10" s="118">
+        <f t="shared" ref="T10" si="23">IFERROR(S10/R10,"")</f>
+        <v>0.21264367816091953</v>
+      </c>
+      <c r="U10" s="123">
+        <v>262927</v>
+      </c>
+      <c r="V10" s="123">
+        <f t="shared" ref="V10" si="24">IFERROR(ROUND(U10*X10,0),"")</f>
+        <v>34181</v>
+      </c>
+      <c r="W10" s="118">
+        <f t="shared" ref="W10" si="25">IFERROR(S10/R10-U10/P10,"")</f>
+        <v>2.1243081232914879E-2</v>
+      </c>
       <c r="X10" s="119">
         <v>0.13</v>
       </c>
-      <c r="Y10" s="170"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="10"/>
+      <c r="Y10" s="297" t="s">
+        <v>2678</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>44977</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:28" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="290"/>
@@ -32741,11 +32796,11 @@
       <c r="S11" s="116"/>
       <c r="T11" s="117"/>
       <c r="U11" s="123" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="U10:U12" si="26">IFERROR(ROUND(P11*S11/R11,0),"")</f>
         <v/>
       </c>
       <c r="V11" s="123" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="V10:V12" si="27">IFERROR(ROUND(U11*X11,0),"")</f>
         <v/>
       </c>
       <c r="W11" s="118"/>
@@ -32778,11 +32833,11 @@
       <c r="S12" s="116"/>
       <c r="T12" s="117"/>
       <c r="U12" s="123" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="V12" s="123" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="W12" s="118"/>
@@ -32957,11 +33012,11 @@
     <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="189">
         <f>SUBTOTAL(109,B2:B17)</f>
-        <v>2885856</v>
+        <v>2985856</v>
       </c>
       <c r="C18" s="189">
         <f>SUBTOTAL(109,C2:C17)</f>
-        <v>375162</v>
+        <v>388662</v>
       </c>
       <c r="D18" s="178" t="s">
         <v>170</v>
@@ -32984,11 +33039,11 @@
       <c r="T18" s="188"/>
       <c r="U18" s="189">
         <f>SUBTOTAL(109,U2:U17)</f>
-        <v>2885856</v>
+        <v>3148783</v>
       </c>
       <c r="V18" s="189">
         <f>SUBTOTAL(109,V2:V17)</f>
-        <v>375162</v>
+        <v>409343</v>
       </c>
       <c r="W18" s="190"/>
       <c r="X18" s="187"/>
@@ -33014,7 +33069,7 @@
       <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A4:AV400" xr:uid="{744AF146-97D6-4F81-B26A-F6968663118F}">
+      <autoFilter ref="A4:AV400" xr:uid="{2D82B068-2772-42C1-AB44-70A0B0E47975}">
         <filterColumn colId="6">
           <filters>
             <filter val="2019.06"/>
@@ -36772,7 +36827,7 @@
       <selection activeCell="L44" sqref="L44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A41:N455" xr:uid="{85C8E3FB-C4D1-4833-8E48-BD1EF47A0B0A}"/>
+      <autoFilter ref="A41:N455" xr:uid="{92164A89-669A-4FD4-9A4B-4DD748EE7D60}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">

</xml_diff>

<commit_message>
no file found fix
</commit_message>
<xml_diff>
--- a/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
+++ b/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felhasználó\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4463D44F-361C-4B16-9AB4-F4E359D80691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDBFDFB-4781-4C19-AB84-998F6C1ED088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25005" yWindow="2025" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terv-tény" sheetId="2" r:id="rId1"/>
@@ -13817,7 +13817,7 @@
       <selection activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-      <autoFilter ref="A3:L77" xr:uid="{EE3C3F08-645C-4296-99D4-DFA922CC3AF5}"/>
+      <autoFilter ref="A3:L77" xr:uid="{8FA59D12-522B-4BF6-AD07-8858A0F7825E}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -33014,7 +33014,7 @@
       <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A4:AV400" xr:uid="{744AF146-97D6-4F81-B26A-F6968663118F}">
+      <autoFilter ref="A4:AV400" xr:uid="{E074E541-6F6D-4540-B945-832E574080A5}">
         <filterColumn colId="6">
           <filters>
             <filter val="2019.06"/>
@@ -36772,7 +36772,7 @@
       <selection activeCell="L44" sqref="L44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A41:N455" xr:uid="{85C8E3FB-C4D1-4833-8E48-BD1EF47A0B0A}"/>
+      <autoFilter ref="A41:N455" xr:uid="{BFE3C56A-017D-4CD5-BBAB-A183EADFB1B1}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">

</xml_diff>

<commit_message>
new generator option implemented
</commit_message>
<xml_diff>
--- a/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
+++ b/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdomj\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2E7B08-B405-46A6-986A-B079C38B4102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C1B57A-1C97-46E5-AD69-2CC3506EA4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terv-tény" sheetId="2" r:id="rId1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8937" uniqueCount="2704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8938" uniqueCount="2704">
   <si>
     <t>Fennmaradó 
 egyenleg</t>
@@ -11237,36 +11237,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -11536,6 +11506,36 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -12140,15 +12140,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07AD6580-3623-47C8-ADC6-6BB1DFD4B47A}" name="admin_feor" displayName="admin_feor" ref="A1:F465" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" headerRowCellStyle="Normál 10" dataCellStyle="Normál 10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07AD6580-3623-47C8-ADC6-6BB1DFD4B47A}" name="admin_feor" displayName="admin_feor" ref="A1:F465" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" headerRowCellStyle="Normál 10" dataCellStyle="Normál 10">
   <autoFilter ref="A1:F465" xr:uid="{134BEC41-0044-4498-9682-8387D48047F7}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4B5B3757-85FD-43F8-9B62-258A51581B25}" name="Foglalkozás" dataDxfId="10" dataCellStyle="Normál 10"/>
-    <tableColumn id="2" xr3:uid="{088A5379-AB2C-41A2-B801-84898C80E47E}" name="Oszlop1" dataDxfId="9" dataCellStyle="Normál 10"/>
-    <tableColumn id="3" xr3:uid="{1F13ABBE-8719-424A-B0CA-9928AA7B7103}" name="Korcsoport" dataDxfId="8" dataCellStyle="Normál 10"/>
-    <tableColumn id="4" xr3:uid="{265CADDD-7107-4B8D-8DDB-287234852308}" name="Oszlop2" dataDxfId="7" dataCellStyle="Normál 10"/>
-    <tableColumn id="5" xr3:uid="{AD8DE1A1-3EAE-482F-81E1-7B13CDE144A8}" name="Oszlop3" dataDxfId="6" dataCellStyle="Normál 10"/>
-    <tableColumn id="6" xr3:uid="{0FDC9587-BA60-4325-A17F-3E74875A154D}" name="Oszlop4" dataDxfId="5" dataCellStyle="Normál 10"/>
+    <tableColumn id="1" xr3:uid="{4B5B3757-85FD-43F8-9B62-258A51581B25}" name="Foglalkozás" dataDxfId="7" dataCellStyle="Normál 10"/>
+    <tableColumn id="2" xr3:uid="{088A5379-AB2C-41A2-B801-84898C80E47E}" name="Oszlop1" dataDxfId="6" dataCellStyle="Normál 10"/>
+    <tableColumn id="3" xr3:uid="{1F13ABBE-8719-424A-B0CA-9928AA7B7103}" name="Korcsoport" dataDxfId="5" dataCellStyle="Normál 10"/>
+    <tableColumn id="4" xr3:uid="{265CADDD-7107-4B8D-8DDB-287234852308}" name="Oszlop2" dataDxfId="4" dataCellStyle="Normál 10"/>
+    <tableColumn id="5" xr3:uid="{AD8DE1A1-3EAE-482F-81E1-7B13CDE144A8}" name="Oszlop3" dataDxfId="3" dataCellStyle="Normál 10"/>
+    <tableColumn id="6" xr3:uid="{0FDC9587-BA60-4325-A17F-3E74875A154D}" name="Oszlop4" dataDxfId="2" dataCellStyle="Normál 10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13817,7 +13817,7 @@
       <selection activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-      <autoFilter ref="A3:L77" xr:uid="{308DB6E6-3B97-4600-8E47-E6469C5F57F1}"/>
+      <autoFilter ref="A3:L77" xr:uid="{2699D51D-345C-40EB-B744-360600ED705E}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -13829,17 +13829,17 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="H3:H25 H29:H36">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12:O14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P8">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31947,9 +31947,9 @@
   <sheetPr codeName="Munka2"/>
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y18" sqref="Y18"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -31990,6 +31990,9 @@
       <c r="C1" s="4" t="s">
         <v>2559</v>
       </c>
+      <c r="E1" s="115" t="s">
+        <v>2561</v>
+      </c>
       <c r="F1" t="s">
         <v>2560</v>
       </c>
@@ -33057,7 +33060,7 @@
       <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A4:AV400" xr:uid="{50F534EF-ABB6-4DD0-B706-F231E7F16358}">
+      <autoFilter ref="A4:AV400" xr:uid="{C9D1B45E-6EDE-4979-BDAD-24DC7F024D13}">
         <filterColumn colId="6">
           <filters>
             <filter val="2019.06"/>
@@ -36815,7 +36818,7 @@
       <selection activeCell="L44" sqref="L44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A41:N455" xr:uid="{9BE863F8-B3C0-4F69-AD6A-1B23F8F88959}"/>
+      <autoFilter ref="A41:N455" xr:uid="{F88C186B-EED0-48F3-8D4B-A52F2CA0DC07}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">

</xml_diff>

<commit_message>
added filter option for month written in text
</commit_message>
<xml_diff>
--- a/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
+++ b/TestApp/bin/Debug/net6.0-windows/Resources/rrf_teszt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdomj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felhasználó\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C1B57A-1C97-46E5-AD69-2CC3506EA4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2E272C-E5F1-41B2-8784-6930C045CD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8938" uniqueCount="2704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8927" uniqueCount="2704">
   <si>
     <t>Fennmaradó 
 egyenleg</t>
@@ -12585,11 +12585,11 @@
       </c>
       <c r="E3" s="295">
         <f>SUMIFS(Bérköltség!$B$2:$B$17,Bérköltség!$K$2:$K$17,$C3,Bérköltség!$N$2:$N$17,"Tény")+SUMIFS(Bérköltség!$C$2:$C$17,Bérköltség!$K$2:$K$17,$C3,Bérköltség!$N$2:$N$17,"Tény")</f>
-        <v>465898</v>
+        <v>352398</v>
       </c>
       <c r="F3" s="295">
         <f>D3-E3</f>
-        <v>460246402</v>
+        <v>460359902</v>
       </c>
       <c r="G3" s="295">
         <f>SUMIFS(Bérköltség!$B$2:$B$17,Bérköltség!$K$2:$K$17,$C3,Bérköltség!$N$2:$N$17,"Köt.váll")+SUMIFS(Bérköltség!$C$2:$C$17,Bérköltség!$K$2:$K$17,$C3,Bérköltség!$N$2:$N$17,"Köt.váll")</f>
@@ -12597,7 +12597,7 @@
       </c>
       <c r="H3" s="133">
         <f>F3-G3</f>
-        <v>458212402</v>
+        <v>458325902</v>
       </c>
       <c r="J3" s="110" t="s">
         <v>129</v>
@@ -12611,11 +12611,11 @@
       </c>
       <c r="M3" s="112">
         <f>SUMIFS(Bérköltség!$B$2:$B$17,Bérköltség!$I$2:$I$17,$K3,Bérköltség!$N$2:$N$17,"Tény")+SUMIFS(Bérköltség!$C$2:$C$17,Bérköltség!$I$2:$I$17,$K3,Bérköltség!$N$2:$N$17,"Tény")+SUMIFS(Dologi_felhalm.!$I$3:$I$84,Dologi_felhalm.!$L$3:$L$84,$K3,Dologi_felhalm.!$J$3:$J$84,"Tény")</f>
-        <v>1364149</v>
+        <v>1250649</v>
       </c>
       <c r="N3" s="112">
         <f>L3-M3</f>
-        <v>240379619</v>
+        <v>240493119</v>
       </c>
       <c r="O3" s="112">
         <f>SUMIFS(Bérköltség!$B$2:$B$17,Bérköltség!$I$2:$I$17,$K3,Bérköltség!$N$2:$N$17,"Köt.váll")+SUMIFS(Bérköltség!$C$2:$C$17,Bérköltség!$I$2:$I$17,$K3,Bérköltség!$N$2:$N$17,"Köt.váll")+SUMIFS(Dologi_felhalm.!$I$3:$I$84,Dologi_felhalm.!$L$3:$L$84,$K3,Dologi_felhalm.!$J$3:$J$84,"Köt.váll")</f>
@@ -12623,7 +12623,7 @@
       </c>
       <c r="P3" s="113">
         <f>N3-O3</f>
-        <v>232117181</v>
+        <v>232230681</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -12889,11 +12889,11 @@
       </c>
       <c r="M8" s="125">
         <f t="shared" ref="M8:P8" si="4">SUM(M3:M7)</f>
-        <v>10525401</v>
+        <v>10411901</v>
       </c>
       <c r="N8" s="125">
         <f t="shared" si="4"/>
-        <v>859474599</v>
+        <v>859588099</v>
       </c>
       <c r="O8" s="125">
         <f t="shared" si="4"/>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="P8" s="126">
         <f t="shared" si="4"/>
-        <v>849302953</v>
+        <v>849416453</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13069,11 +13069,11 @@
       </c>
       <c r="L12" s="168">
         <f t="shared" ref="L12:O12" si="5">SUM(E25)</f>
-        <v>9302087</v>
+        <v>9188587</v>
       </c>
       <c r="M12" s="167">
         <f t="shared" si="5"/>
-        <v>785122948</v>
+        <v>785236448</v>
       </c>
       <c r="N12" s="167">
         <f t="shared" si="5"/>
@@ -13081,7 +13081,7 @@
       </c>
       <c r="O12" s="169">
         <f t="shared" si="5"/>
-        <v>775291885</v>
+        <v>775405385</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -13178,11 +13178,11 @@
       </c>
       <c r="L14" s="293">
         <f t="shared" ref="L14:O14" si="7">SUM(L12:L13)</f>
-        <v>10525401</v>
+        <v>10411901</v>
       </c>
       <c r="M14" s="109">
         <f t="shared" si="7"/>
-        <v>859474599</v>
+        <v>859588099</v>
       </c>
       <c r="N14" s="293">
         <f t="shared" si="7"/>
@@ -13190,7 +13190,7 @@
       </c>
       <c r="O14" s="294">
         <f t="shared" si="7"/>
-        <v>849302953</v>
+        <v>849416453</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
@@ -13516,11 +13516,11 @@
       </c>
       <c r="E25" s="58">
         <f t="shared" ref="E25:H25" si="8">SUM(E3:E24)</f>
-        <v>9302087</v>
+        <v>9188587</v>
       </c>
       <c r="F25" s="58">
         <f t="shared" si="8"/>
-        <v>785122948</v>
+        <v>785236448</v>
       </c>
       <c r="G25" s="58">
         <f t="shared" si="8"/>
@@ -13528,7 +13528,7 @@
       </c>
       <c r="H25" s="58">
         <f t="shared" si="8"/>
-        <v>775291885</v>
+        <v>775405385</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -13817,7 +13817,7 @@
       <selection activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-      <autoFilter ref="A3:L77" xr:uid="{2699D51D-345C-40EB-B744-360600ED705E}"/>
+      <autoFilter ref="A3:L77" xr:uid="{CEDA9C96-4C70-46CB-96E9-E2A219CA817C}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -31949,7 +31949,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -32602,7 +32602,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="236">
-        <v>8346442386</v>
+        <v>8427102364</v>
       </c>
       <c r="F9" s="35" t="s">
         <v>172</v>
@@ -32676,94 +32676,42 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="291" t="e">
-        <f>IF(#REF!="FEOR",#REF!,IF(#REF!="HIÁNYOS ADATOK","HIÁNYOS ADATOK",#REF!))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B10" s="256">
-        <v>100000</v>
-      </c>
-      <c r="C10" s="256">
-        <v>13500</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="236">
-        <v>8346442386</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>1215</v>
-      </c>
-      <c r="G10" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="L10" s="81" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="108" t="str">
-        <f>IF(COUNTIFS(Admin!$A$29:$A$40,L10)&gt;0,Admin!$A$28,IF(COUNTIFS(Admin!$B$29:$B$40,L10)&gt;0,Admin!$B$28,IF(COUNTIFS(Admin!$C$29:$C$40,L10)&gt;0,Admin!$C$28,IF(COUNTIFS(Admin!$D$29:$D$40,L10)&gt;0,Admin!$D$28,"-"))))</f>
-        <v>2. mérföldkő</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="P10" s="121">
-        <v>1373700</v>
-      </c>
-      <c r="Q10" s="122">
-        <f t="shared" ref="Q10" si="22">IFERROR(ROUND(P10*X10,0),"")</f>
-        <v>178581</v>
-      </c>
-      <c r="R10" s="116">
-        <v>174</v>
-      </c>
-      <c r="S10" s="116">
-        <v>37</v>
-      </c>
-      <c r="T10" s="118">
-        <f t="shared" ref="T10" si="23">IFERROR(S10/R10,"")</f>
-        <v>0.21264367816091953</v>
-      </c>
-      <c r="U10" s="123">
-        <v>262927</v>
-      </c>
-      <c r="V10" s="123">
-        <f t="shared" ref="V10" si="24">IFERROR(ROUND(U10*X10,0),"")</f>
-        <v>34181</v>
-      </c>
-      <c r="W10" s="118">
-        <f t="shared" ref="W10" si="25">IFERROR(S10/R10-U10/P10,"")</f>
-        <v>2.1243081232914879E-2</v>
-      </c>
+    <row r="10" spans="1:28" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="290"/>
+      <c r="B10" s="256"/>
+      <c r="C10" s="256"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="265"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="108"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="121"/>
+      <c r="Q10" s="122"/>
+      <c r="R10" s="116"/>
+      <c r="S10" s="116"/>
+      <c r="T10" s="117"/>
+      <c r="U10" s="123" t="str">
+        <f t="shared" ref="U10:U12" si="22">IFERROR(ROUND(P10*S10/R10,0),"")</f>
+        <v/>
+      </c>
+      <c r="V10" s="123" t="str">
+        <f t="shared" ref="V10:V12" si="23">IFERROR(ROUND(U10*X10,0),"")</f>
+        <v/>
+      </c>
+      <c r="W10" s="118"/>
       <c r="X10" s="119">
         <v>0.13</v>
       </c>
-      <c r="Y10" s="297" t="s">
-        <v>2678</v>
-      </c>
-      <c r="Z10" s="12">
-        <v>44977</v>
-      </c>
-      <c r="AA10" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="Y10" s="170"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="10"/>
     </row>
     <row r="11" spans="1:28" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="290"/>
@@ -32787,11 +32735,11 @@
       <c r="S11" s="116"/>
       <c r="T11" s="117"/>
       <c r="U11" s="123" t="str">
-        <f t="shared" ref="U11:U12" si="26">IFERROR(ROUND(P11*S11/R11,0),"")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="V11" s="123" t="str">
-        <f t="shared" ref="V11:V12" si="27">IFERROR(ROUND(U11*X11,0),"")</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="W11" s="118"/>
@@ -32824,11 +32772,11 @@
       <c r="S12" s="116"/>
       <c r="T12" s="117"/>
       <c r="U12" s="123" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="V12" s="123" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="W12" s="118"/>
@@ -33003,11 +32951,11 @@
     <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="189">
         <f>SUBTOTAL(109,B2:B17)</f>
-        <v>2985856</v>
+        <v>2885856</v>
       </c>
       <c r="C18" s="189">
         <f>SUBTOTAL(109,C2:C17)</f>
-        <v>388662</v>
+        <v>375162</v>
       </c>
       <c r="D18" s="178" t="s">
         <v>170</v>
@@ -33030,11 +32978,11 @@
       <c r="T18" s="188"/>
       <c r="U18" s="189">
         <f>SUBTOTAL(109,U2:U17)</f>
-        <v>3148783</v>
+        <v>2885856</v>
       </c>
       <c r="V18" s="189">
         <f>SUBTOTAL(109,V2:V17)</f>
-        <v>409343</v>
+        <v>375162</v>
       </c>
       <c r="W18" s="190"/>
       <c r="X18" s="187"/>
@@ -33060,7 +33008,7 @@
       <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A4:AV400" xr:uid="{C9D1B45E-6EDE-4979-BDAD-24DC7F024D13}">
+      <autoFilter ref="A4:AV400" xr:uid="{4BFD3475-F5DE-4495-B6CC-CB5264DDC443}">
         <filterColumn colId="6">
           <filters>
             <filter val="2019.06"/>
@@ -36818,7 +36766,7 @@
       <selection activeCell="L44" sqref="L44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A41:N455" xr:uid="{F88C186B-EED0-48F3-8D4B-A52F2CA0DC07}"/>
+      <autoFilter ref="A41:N455" xr:uid="{CDD8AAF9-DE00-4853-A30A-AE962968774F}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">

</xml_diff>